<commit_message>
Added the correct presets in the timesheettemplate and the timesheet template dummy
</commit_message>
<xml_diff>
--- a/TimesheetTemplate.xlsx
+++ b/TimesheetTemplate.xlsx
@@ -2226,7 +2226,10 @@
       <c r="G15" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="38"/>
+      <c r="H15" s="38">
+        <f>B33+1</f>
+        <v>7</v>
+      </c>
       <c r="I15" s="41"/>
       <c r="J15" s="42"/>
       <c r="K15" s="28"/>
@@ -2306,7 +2309,10 @@
       <c r="A18" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="38"/>
+      <c r="B18" s="38">
+        <f>B15+1</f>
+        <v>1</v>
+      </c>
       <c r="C18" s="39"/>
       <c r="D18" s="22"/>
       <c r="E18" s="40"/>
@@ -2314,7 +2320,10 @@
       <c r="G18" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="38"/>
+      <c r="H18" s="38">
+        <f>H15+1</f>
+        <v>8</v>
+      </c>
       <c r="I18" s="41"/>
       <c r="J18" s="42"/>
       <c r="K18" s="28"/>
@@ -2394,7 +2403,10 @@
       <c r="A21" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="38"/>
+      <c r="B21" s="38">
+        <f>B18+1</f>
+        <v>2</v>
+      </c>
       <c r="C21" s="39"/>
       <c r="D21" s="22"/>
       <c r="E21" s="40"/>
@@ -2402,7 +2414,10 @@
       <c r="G21" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="38"/>
+      <c r="H21" s="38">
+        <f>H18+1</f>
+        <v>9</v>
+      </c>
       <c r="I21" s="52"/>
       <c r="J21" s="42"/>
       <c r="K21" s="28"/>
@@ -2482,7 +2497,10 @@
       <c r="A24" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="38"/>
+      <c r="B24" s="38">
+        <f>B21+1</f>
+        <v>3</v>
+      </c>
       <c r="C24" s="39"/>
       <c r="D24" s="22"/>
       <c r="E24" s="40"/>
@@ -2490,7 +2508,10 @@
       <c r="G24" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="H24" s="38"/>
+      <c r="H24" s="38">
+        <f>H21+1</f>
+        <v>10</v>
+      </c>
       <c r="I24" s="41"/>
       <c r="J24" s="42"/>
       <c r="K24" s="28"/>
@@ -2570,7 +2591,10 @@
       <c r="A27" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="38"/>
+      <c r="B27" s="38">
+        <f>B24+1</f>
+        <v>4</v>
+      </c>
       <c r="C27" s="39"/>
       <c r="D27" s="22"/>
       <c r="E27" s="40"/>
@@ -2578,7 +2602,10 @@
       <c r="G27" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="38"/>
+      <c r="H27" s="38">
+        <f>H24+1</f>
+        <v>11</v>
+      </c>
       <c r="I27" s="54"/>
       <c r="J27" s="42"/>
       <c r="K27" s="28"/>
@@ -2658,7 +2685,10 @@
       <c r="A30" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="56"/>
+      <c r="B30" s="56">
+        <f>B27+1</f>
+        <v>5</v>
+      </c>
       <c r="C30" s="57"/>
       <c r="D30" s="58"/>
       <c r="E30" s="40"/>
@@ -2666,7 +2696,10 @@
       <c r="G30" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H30" s="56"/>
+      <c r="H30" s="56">
+        <f>H27+1</f>
+        <v>12</v>
+      </c>
       <c r="I30" s="59"/>
       <c r="J30" s="42"/>
       <c r="K30" s="28"/>
@@ -2746,7 +2779,10 @@
       <c r="A33" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="56"/>
+      <c r="B33" s="56">
+        <f>B30+1</f>
+        <v>6</v>
+      </c>
       <c r="C33" s="57"/>
       <c r="D33" s="58"/>
       <c r="E33" s="66"/>

</xml_diff>

<commit_message>
Added the homescreen, setname, setTimesheetPeriod, and the File Rename function for the excel
</commit_message>
<xml_diff>
--- a/TimesheetTemplate.xlsx
+++ b/TimesheetTemplate.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>ESCALATE LIFE SCIENCES</t>
   </si>
@@ -50,9 +50,6 @@
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
-  </si>
-  <si>
-    <t>Ricardo Rios</t>
   </si>
   <si>
     <t>Client Name:</t>
@@ -226,7 +223,7 @@
     <t>RATE</t>
   </si>
   <si>
-    <t>55/hr</t>
+    <t>50/hr</t>
   </si>
   <si>
     <t xml:space="preserve">Fax: </t>
@@ -1190,7 +1187,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="183">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1276,8 +1273,8 @@
     <xf borderId="22" fillId="0" fontId="7" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="9" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="2" fontId="6" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
@@ -1297,6 +1294,9 @@
     <xf borderId="30" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="31" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="32" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="2" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="11" fillId="2" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -1438,7 +1438,7 @@
     </xf>
     <xf borderId="3" fillId="2" fontId="19" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="21" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="167" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="20" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -1900,7 +1900,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" ht="12.75" customHeight="1">
+    <row r="2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1931,7 +1931,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" ht="12.75" customHeight="1">
+    <row r="5">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1957,17 +1957,15 @@
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="9"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>9</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="11"/>
@@ -1989,18 +1987,18 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>11</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>13</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -2022,7 +2020,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="14">
         <v>45537.0</v>
@@ -2031,7 +2029,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="2"/>
@@ -2054,7 +2052,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="16">
         <v>45550.0</v>
@@ -2063,7 +2061,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="2"/>
@@ -2087,7 +2085,7 @@
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="18"/>
       <c r="B11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="19">
         <v>45551.0</v>
@@ -2097,7 +2095,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="2"/>
@@ -2148,26 +2146,26 @@
     </row>
     <row r="13" ht="15.0" customHeight="1">
       <c r="A13" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="22"/>
       <c r="C13" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K13" s="28"/>
       <c r="L13" s="2"/>
@@ -2216,7 +2214,7 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="38"/>
       <c r="C15" s="39"/>
@@ -2224,7 +2222,7 @@
       <c r="E15" s="40"/>
       <c r="F15" s="25"/>
       <c r="G15" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="38">
         <f>B33+1</f>
@@ -2307,18 +2305,18 @@
     </row>
     <row r="18" ht="17.25" customHeight="1">
       <c r="A18" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="38">
         <f>B15+1</f>
         <v>1</v>
       </c>
-      <c r="C18" s="39"/>
+      <c r="C18" s="52"/>
       <c r="D18" s="22"/>
       <c r="E18" s="40"/>
       <c r="F18" s="25"/>
       <c r="G18" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H18" s="38">
         <f>H15+1</f>
@@ -2401,24 +2399,24 @@
     </row>
     <row r="21" ht="17.25" customHeight="1">
       <c r="A21" s="37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="38">
         <f>B18+1</f>
         <v>2</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="22"/>
       <c r="E21" s="40"/>
       <c r="F21" s="25"/>
       <c r="G21" s="37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H21" s="38">
         <f>H18+1</f>
         <v>9</v>
       </c>
-      <c r="I21" s="52"/>
+      <c r="I21" s="53"/>
       <c r="J21" s="42"/>
       <c r="K21" s="28"/>
       <c r="L21" s="2"/>
@@ -2446,7 +2444,7 @@
       <c r="F22" s="25"/>
       <c r="G22" s="43"/>
       <c r="H22" s="44"/>
-      <c r="I22" s="53"/>
+      <c r="I22" s="54"/>
       <c r="J22" s="33"/>
       <c r="K22" s="36"/>
       <c r="L22" s="2"/>
@@ -2495,18 +2493,18 @@
     </row>
     <row r="24" ht="17.25" customHeight="1">
       <c r="A24" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="38">
         <f>B21+1</f>
         <v>3</v>
       </c>
-      <c r="C24" s="39"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="22"/>
       <c r="E24" s="40"/>
       <c r="F24" s="25"/>
       <c r="G24" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H24" s="38">
         <f>H21+1</f>
@@ -2589,24 +2587,24 @@
     </row>
     <row r="27" ht="17.25" customHeight="1">
       <c r="A27" s="37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="38">
         <f>B24+1</f>
         <v>4</v>
       </c>
-      <c r="C27" s="39"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="22"/>
       <c r="E27" s="40"/>
       <c r="F27" s="25"/>
       <c r="G27" s="37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H27" s="38">
         <f>H24+1</f>
         <v>11</v>
       </c>
-      <c r="I27" s="54"/>
+      <c r="I27" s="55"/>
       <c r="J27" s="42"/>
       <c r="K27" s="28"/>
       <c r="L27" s="2"/>
@@ -2662,7 +2660,7 @@
       <c r="F29" s="25"/>
       <c r="G29" s="48"/>
       <c r="H29" s="49"/>
-      <c r="I29" s="55"/>
+      <c r="I29" s="56"/>
       <c r="J29" s="29"/>
       <c r="K29" s="51"/>
       <c r="L29" s="2"/>
@@ -2683,24 +2681,24 @@
     </row>
     <row r="30" ht="30.0" customHeight="1">
       <c r="A30" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="56">
+        <v>28</v>
+      </c>
+      <c r="B30" s="57">
         <f>B27+1</f>
         <v>5</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59"/>
       <c r="E30" s="40"/>
       <c r="F30" s="25"/>
       <c r="G30" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="56">
+        <v>28</v>
+      </c>
+      <c r="H30" s="57">
         <f>H27+1</f>
         <v>12</v>
       </c>
-      <c r="I30" s="59"/>
+      <c r="I30" s="60"/>
       <c r="J30" s="42"/>
       <c r="K30" s="28"/>
       <c r="L30" s="2"/>
@@ -2722,13 +2720,13 @@
     <row r="31" ht="8.25" customHeight="1">
       <c r="A31" s="43"/>
       <c r="B31" s="44"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="62"/>
       <c r="E31" s="46"/>
       <c r="F31" s="25"/>
       <c r="G31" s="43"/>
       <c r="H31" s="44"/>
-      <c r="I31" s="62"/>
+      <c r="I31" s="63"/>
       <c r="J31" s="33"/>
       <c r="K31" s="36"/>
       <c r="L31" s="2"/>
@@ -2750,13 +2748,13 @@
     <row r="32" ht="9.75" customHeight="1">
       <c r="A32" s="48"/>
       <c r="B32" s="49"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="32"/>
       <c r="F32" s="25"/>
       <c r="G32" s="48"/>
       <c r="H32" s="49"/>
-      <c r="I32" s="65"/>
+      <c r="I32" s="66"/>
       <c r="J32" s="29"/>
       <c r="K32" s="51"/>
       <c r="L32" s="2"/>
@@ -2777,21 +2775,21 @@
     </row>
     <row r="33" ht="17.25" customHeight="1">
       <c r="A33" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="56">
+        <v>29</v>
+      </c>
+      <c r="B33" s="57">
         <f>B30+1</f>
         <v>6</v>
       </c>
-      <c r="C33" s="57"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="66"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="67"/>
       <c r="F33" s="25"/>
       <c r="G33" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="H33" s="56"/>
-      <c r="I33" s="59"/>
+        <v>29</v>
+      </c>
+      <c r="H33" s="57"/>
+      <c r="I33" s="60"/>
       <c r="J33" s="42"/>
       <c r="K33" s="28"/>
       <c r="L33" s="2"/>
@@ -2813,13 +2811,13 @@
     <row r="34" ht="21.0" customHeight="1">
       <c r="A34" s="43"/>
       <c r="B34" s="44"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="61"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="62"/>
       <c r="E34" s="46"/>
       <c r="F34" s="25"/>
       <c r="G34" s="43"/>
       <c r="H34" s="44"/>
-      <c r="I34" s="62"/>
+      <c r="I34" s="63"/>
       <c r="J34" s="33"/>
       <c r="K34" s="36"/>
       <c r="L34" s="2"/>
@@ -2841,13 +2839,13 @@
     <row r="35" ht="6.75" customHeight="1">
       <c r="A35" s="43"/>
       <c r="B35" s="49"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="65"/>
       <c r="E35" s="46"/>
       <c r="F35" s="25"/>
       <c r="G35" s="43"/>
       <c r="H35" s="49"/>
-      <c r="I35" s="65"/>
+      <c r="I35" s="66"/>
       <c r="J35" s="29"/>
       <c r="K35" s="51"/>
       <c r="L35" s="2"/>
@@ -2868,27 +2866,27 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
+        <v>30</v>
+      </c>
+      <c r="B36" s="68"/>
+      <c r="C36" s="68"/>
       <c r="D36" s="22"/>
-      <c r="E36" s="68">
+      <c r="E36" s="69">
         <f>SUM(E15:E35)</f>
         <v>0</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H36" s="67"/>
-      <c r="I36" s="67"/>
-      <c r="J36" s="69">
+        <v>30</v>
+      </c>
+      <c r="H36" s="68"/>
+      <c r="I36" s="68"/>
+      <c r="J36" s="70">
         <f>SUM(J15:J35)</f>
         <v>0</v>
       </c>
-      <c r="K36" s="67"/>
-      <c r="L36" s="70"/>
+      <c r="K36" s="68"/>
+      <c r="L36" s="71"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -2906,17 +2904,17 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="29"/>
-      <c r="B37" s="71"/>
-      <c r="C37" s="71"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
       <c r="D37" s="30"/>
       <c r="E37" s="32"/>
       <c r="F37" s="25"/>
       <c r="G37" s="29"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="71"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="72"/>
       <c r="J37" s="29"/>
-      <c r="K37" s="71"/>
-      <c r="L37" s="70"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="71"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -2934,7 +2932,7 @@
     </row>
     <row r="38" ht="18.75" customHeight="1">
       <c r="A38" s="25"/>
-      <c r="B38" s="72"/>
+      <c r="B38" s="73"/>
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
@@ -2959,22 +2957,22 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39" ht="28.5" customHeight="1">
-      <c r="A39" s="73"/>
-      <c r="B39" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="75"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="76" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" s="77"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="79">
+      <c r="A39" s="74"/>
+      <c r="B39" s="75" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="76"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="78"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="80">
         <f>E36+J36</f>
         <v>0</v>
       </c>
-      <c r="I39" s="73"/>
+      <c r="I39" s="74"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="2"/>
@@ -2994,21 +2992,21 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" ht="16.5" customHeight="1">
-      <c r="A40" s="73"/>
-      <c r="B40" s="80" t="s">
+      <c r="A40" s="74"/>
+      <c r="B40" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="81" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" s="73"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="82"/>
-      <c r="G40" s="82"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="73"/>
-      <c r="J40" s="73"/>
-      <c r="K40" s="73"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="84"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="74"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -3027,18 +3025,18 @@
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="4"/>
-      <c r="B41" s="84"/>
+      <c r="B41" s="85"/>
       <c r="C41" s="5"/>
       <c r="D41" s="2"/>
       <c r="E41" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F41" s="73"/>
-      <c r="G41" s="73"/>
+        <v>34</v>
+      </c>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="73"/>
-      <c r="K41" s="73"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="74"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3057,8 +3055,8 @@
     </row>
     <row r="42" ht="25.5" customHeight="1">
       <c r="A42" s="2"/>
-      <c r="B42" s="85"/>
-      <c r="C42" s="85"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="86"/>
       <c r="D42" s="25"/>
       <c r="E42" s="25"/>
       <c r="F42" s="25"/>
@@ -3086,15 +3084,15 @@
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="25"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="85"/>
-      <c r="D43" s="86" t="s">
-        <v>36</v>
-      </c>
-      <c r="E43" s="87"/>
-      <c r="F43" s="87"/>
-      <c r="G43" s="87"/>
-      <c r="H43" s="87"/>
-      <c r="I43" s="87"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="87" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="88"/>
+      <c r="F43" s="88"/>
+      <c r="G43" s="88"/>
+      <c r="H43" s="88"/>
+      <c r="I43" s="88"/>
       <c r="J43" s="25"/>
       <c r="K43" s="25"/>
       <c r="L43" s="2"/>
@@ -3116,16 +3114,16 @@
     <row r="44" ht="50.25" customHeight="1">
       <c r="A44" s="25"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="85"/>
-      <c r="D44" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="E44" s="88"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" s="89"/>
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
-      <c r="I44" s="89" t="s">
-        <v>38</v>
+      <c r="I44" s="90" t="s">
+        <v>37</v>
       </c>
       <c r="J44" s="25"/>
       <c r="K44" s="25"/>
@@ -3148,13 +3146,13 @@
     <row r="45" ht="23.25" customHeight="1">
       <c r="A45" s="25"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="85"/>
-      <c r="D45" s="90"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="90"/>
-      <c r="H45" s="90"/>
-      <c r="I45" s="90"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="91"/>
+      <c r="E45" s="91"/>
+      <c r="F45" s="91"/>
+      <c r="G45" s="91"/>
+      <c r="H45" s="91"/>
+      <c r="I45" s="91"/>
       <c r="J45" s="25"/>
       <c r="K45" s="25"/>
       <c r="L45" s="2"/>
@@ -3176,13 +3174,13 @@
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="25"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="85"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="72"/>
-      <c r="H46" s="72"/>
-      <c r="I46" s="72"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73"/>
+      <c r="I46" s="73"/>
       <c r="J46" s="25"/>
       <c r="K46" s="25"/>
       <c r="L46" s="2"/>
@@ -3204,13 +3202,13 @@
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="25"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="85"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="72"/>
-      <c r="G47" s="72"/>
-      <c r="H47" s="72"/>
-      <c r="I47" s="72"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="73"/>
+      <c r="E47" s="73"/>
+      <c r="F47" s="73"/>
+      <c r="G47" s="73"/>
+      <c r="H47" s="73"/>
+      <c r="I47" s="73"/>
       <c r="J47" s="25"/>
       <c r="K47" s="25"/>
       <c r="L47" s="2"/>
@@ -3232,9 +3230,9 @@
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="25"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="85"/>
-      <c r="D48" s="91" t="s">
-        <v>39</v>
+      <c r="C48" s="86"/>
+      <c r="D48" s="92" t="s">
+        <v>38</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -3254,7 +3252,7 @@
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="25"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="85"/>
+      <c r="C49" s="86"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -3273,7 +3271,7 @@
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="25"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="85"/>
+      <c r="C50" s="86"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -3291,16 +3289,16 @@
     </row>
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="2"/>
-      <c r="B51" s="92"/>
-      <c r="C51" s="93"/>
-      <c r="D51" s="94"/>
-      <c r="E51" s="92"/>
+      <c r="B51" s="93"/>
+      <c r="C51" s="94"/>
+      <c r="D51" s="95"/>
+      <c r="E51" s="93"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="92"/>
-      <c r="H51" s="92"/>
-      <c r="I51" s="92"/>
-      <c r="J51" s="92"/>
-      <c r="K51" s="92"/>
+      <c r="G51" s="93"/>
+      <c r="H51" s="93"/>
+      <c r="I51" s="93"/>
+      <c r="J51" s="93"/>
+      <c r="K51" s="93"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -3318,7 +3316,7 @@
       <c r="Z51" s="2"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="B52" s="92"/>
+      <c r="B52" s="93"/>
     </row>
     <row r="53" ht="12.75" customHeight="1"/>
     <row r="54" ht="12.75" customHeight="1"/>
@@ -4389,271 +4387,274 @@
   </cols>
   <sheetData>
     <row r="1" ht="48.75" customHeight="1">
-      <c r="A1" s="95"/>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98" t="s">
+      <c r="A1" s="96"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="100"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="96"/>
+      <c r="Y1" s="96"/>
+      <c r="Z1" s="96"/>
+    </row>
+    <row r="2" ht="45.0" customHeight="1">
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="96"/>
+      <c r="Z2" s="96"/>
+    </row>
+    <row r="3" ht="15.0" customHeight="1">
+      <c r="A3" s="96"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="99"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
-      <c r="S1" s="95"/>
-      <c r="T1" s="95"/>
-      <c r="U1" s="95"/>
-      <c r="V1" s="95"/>
-      <c r="W1" s="95"/>
-      <c r="X1" s="95"/>
-      <c r="Y1" s="95"/>
-      <c r="Z1" s="95"/>
-    </row>
-    <row r="2" ht="45.0" customHeight="1">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="95"/>
-      <c r="R2" s="95"/>
-      <c r="S2" s="95"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="95"/>
-      <c r="V2" s="95"/>
-      <c r="W2" s="95"/>
-      <c r="X2" s="95"/>
-      <c r="Y2" s="95"/>
-      <c r="Z2" s="95"/>
-    </row>
-    <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="104" t="s">
+      <c r="E3" s="106" t="str">
+        <f>Timesheet!C7</f>
+        <v/>
+      </c>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="96"/>
+      <c r="R3" s="96"/>
+      <c r="S3" s="96"/>
+      <c r="T3" s="96"/>
+      <c r="U3" s="96"/>
+      <c r="V3" s="96"/>
+      <c r="W3" s="96"/>
+      <c r="X3" s="96"/>
+      <c r="Y3" s="96"/>
+      <c r="Z3" s="96"/>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="D4" s="107" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="105" t="str">
-        <f>Timesheet!C7</f>
-        <v>Ricardo Rios</v>
-      </c>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="95"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="95"/>
-      <c r="X3" s="95"/>
-      <c r="Y3" s="95"/>
-      <c r="Z3" s="95"/>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="D4" s="106" t="s">
+      <c r="E4" s="108"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="109" t="s">
+      <c r="H4" s="111"/>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="D5" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="110"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="D5" s="106" t="s">
+      <c r="E5" s="108"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="107"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="109" t="s">
+      <c r="H5" s="113"/>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="D6" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="112"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="D6" s="106" t="s">
+      <c r="E6" s="114"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="113"/>
-      <c r="F6" s="111"/>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="114" t="s">
+      <c r="I6" s="116"/>
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="D7" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="115"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="D7" s="106" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="107" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="109"/>
-      <c r="I7" s="116"/>
+      <c r="E7" s="108" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="110"/>
+      <c r="I7" s="117"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="117" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="117"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="119"/>
+      <c r="D8" s="118" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="118"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="120"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="D9" s="120"/>
-      <c r="E9" s="121"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="122"/>
       <c r="F9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="123"/>
+      <c r="I9" s="123"/>
+    </row>
+    <row r="10" ht="12.75" customHeight="1">
+      <c r="D10" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="122"/>
-      <c r="I9" s="122"/>
-    </row>
-    <row r="10" ht="12.75" customHeight="1">
-      <c r="D10" s="117" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="123"/>
-      <c r="F10" s="124">
+      <c r="E10" s="124"/>
+      <c r="F10" s="125">
         <f>Timesheet!C9</f>
         <v>45537</v>
       </c>
-      <c r="G10" s="125"/>
-      <c r="H10" s="122"/>
-      <c r="J10" s="122"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="123"/>
+      <c r="J10" s="123"/>
     </row>
     <row r="11" ht="7.5" customHeight="1">
-      <c r="D11" s="120"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="126"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="127"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="122"/>
-      <c r="I11" s="122"/>
+      <c r="H11" s="123"/>
+      <c r="I11" s="123"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="D12" s="117" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="123"/>
-      <c r="F12" s="124">
+      <c r="D12" s="118" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="124"/>
+      <c r="F12" s="125">
         <f>Timesheet!C10</f>
         <v>45550</v>
       </c>
-      <c r="G12" s="125"/>
-      <c r="H12" s="122"/>
-      <c r="I12" s="122"/>
+      <c r="G12" s="126"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
     </row>
     <row r="13" ht="8.25" customHeight="1">
-      <c r="I13" s="127"/>
-      <c r="J13" s="122"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="123"/>
     </row>
     <row r="14" ht="5.25" customHeight="1">
-      <c r="D14" s="128"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="111"/>
-      <c r="H14" s="111"/>
-      <c r="I14" s="127"/>
-      <c r="J14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="112"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="130"/>
     </row>
     <row r="15" ht="25.5" customHeight="1">
-      <c r="A15" s="95"/>
-      <c r="B15" s="130" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="131"/>
-      <c r="D15" s="132" t="s">
+      <c r="A15" s="96"/>
+      <c r="B15" s="131" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="132"/>
+      <c r="D15" s="133" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="134" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="133" t="s">
+      <c r="F15" s="135"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="135"/>
+      <c r="I15" s="136" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="137" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="134"/>
-      <c r="G15" s="134"/>
-      <c r="H15" s="134"/>
-      <c r="I15" s="135" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="136" t="s">
-        <v>56</v>
-      </c>
-      <c r="K15" s="95"/>
-      <c r="L15" s="95"/>
-      <c r="M15" s="95"/>
-      <c r="N15" s="95"/>
-      <c r="O15" s="95"/>
-      <c r="P15" s="95"/>
-      <c r="Q15" s="95"/>
-      <c r="R15" s="95"/>
-      <c r="S15" s="95"/>
-      <c r="T15" s="95"/>
-      <c r="U15" s="95"/>
-      <c r="V15" s="95"/>
-      <c r="W15" s="95"/>
-      <c r="X15" s="95"/>
-      <c r="Y15" s="95"/>
-      <c r="Z15" s="95"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="96"/>
+      <c r="O15" s="96"/>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="96"/>
+      <c r="R15" s="96"/>
+      <c r="S15" s="96"/>
+      <c r="T15" s="96"/>
+      <c r="U15" s="96"/>
+      <c r="V15" s="96"/>
+      <c r="W15" s="96"/>
+      <c r="X15" s="96"/>
+      <c r="Y15" s="96"/>
+      <c r="Z15" s="96"/>
     </row>
     <row r="16" ht="32.25" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="137" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="138">
+      <c r="B16" s="138" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="139">
         <f>F10</f>
         <v>45537</v>
       </c>
-      <c r="D16" s="139"/>
-      <c r="E16" s="140" t="str">
+      <c r="D16" s="140" t="str">
+        <f>Timesheet!E15</f>
+        <v/>
+      </c>
+      <c r="E16" s="141" t="str">
         <f>Timesheet!C15</f>
         <v/>
       </c>
-      <c r="F16" s="134"/>
-      <c r="G16" s="134"/>
-      <c r="H16" s="131"/>
-      <c r="I16" s="141">
+      <c r="F16" s="135"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="132"/>
+      <c r="I16" s="142">
         <v>50.0</v>
       </c>
-      <c r="J16" s="142">
+      <c r="J16" s="143">
         <f t="shared" ref="J16:J29" si="1">I16*D16</f>
         <v>0</v>
       </c>
@@ -4676,28 +4677,28 @@
     </row>
     <row r="17" ht="20.25" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="137" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="138">
+      <c r="B17" s="138" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="139">
         <f t="shared" ref="C17:C29" si="2">C16+1</f>
         <v>45538</v>
       </c>
-      <c r="D17" s="139" t="str">
+      <c r="D17" s="140" t="str">
         <f>Timesheet!E18</f>
         <v/>
       </c>
-      <c r="E17" s="140" t="str">
+      <c r="E17" s="141" t="str">
         <f>Timesheet!C18</f>
         <v/>
       </c>
-      <c r="F17" s="134"/>
-      <c r="G17" s="134"/>
-      <c r="H17" s="131"/>
-      <c r="I17" s="141">
+      <c r="F17" s="135"/>
+      <c r="G17" s="135"/>
+      <c r="H17" s="132"/>
+      <c r="I17" s="142">
         <v>50.0</v>
       </c>
-      <c r="J17" s="142">
+      <c r="J17" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4720,28 +4721,28 @@
     </row>
     <row r="18" ht="22.5" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="137" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="138">
+      <c r="B18" s="138" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="139">
         <f t="shared" si="2"/>
         <v>45539</v>
       </c>
-      <c r="D18" s="139" t="str">
+      <c r="D18" s="140" t="str">
         <f>Timesheet!E21</f>
         <v/>
       </c>
-      <c r="E18" s="140" t="str">
+      <c r="E18" s="141" t="str">
         <f>Timesheet!C21</f>
         <v/>
       </c>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="131"/>
-      <c r="I18" s="141">
+      <c r="F18" s="135"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="132"/>
+      <c r="I18" s="142">
         <v>50.0</v>
       </c>
-      <c r="J18" s="142">
+      <c r="J18" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4764,28 +4765,28 @@
     </row>
     <row r="19" ht="18.0" customHeight="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="137" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="138">
+      <c r="B19" s="138" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="139">
         <f t="shared" si="2"/>
         <v>45540</v>
       </c>
-      <c r="D19" s="139" t="str">
+      <c r="D19" s="140" t="str">
         <f>Timesheet!E24</f>
         <v/>
       </c>
-      <c r="E19" s="140" t="str">
+      <c r="E19" s="141" t="str">
         <f>Timesheet!C24</f>
         <v/>
       </c>
-      <c r="F19" s="134"/>
-      <c r="G19" s="134"/>
-      <c r="H19" s="131"/>
-      <c r="I19" s="141">
+      <c r="F19" s="135"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="132"/>
+      <c r="I19" s="142">
         <v>50.0</v>
       </c>
-      <c r="J19" s="142">
+      <c r="J19" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4808,28 +4809,28 @@
     </row>
     <row r="20" ht="20.25" customHeight="1">
       <c r="A20" s="2"/>
-      <c r="B20" s="137" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="138">
+      <c r="B20" s="138" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="139">
         <f t="shared" si="2"/>
         <v>45541</v>
       </c>
-      <c r="D20" s="139" t="str">
+      <c r="D20" s="140" t="str">
         <f>Timesheet!E27</f>
         <v/>
       </c>
-      <c r="E20" s="140" t="str">
+      <c r="E20" s="141" t="str">
         <f>Timesheet!C27</f>
         <v/>
       </c>
-      <c r="F20" s="134"/>
-      <c r="G20" s="134"/>
-      <c r="H20" s="131"/>
-      <c r="I20" s="141">
+      <c r="F20" s="135"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="132"/>
+      <c r="I20" s="142">
         <v>50.0</v>
       </c>
-      <c r="J20" s="142">
+      <c r="J20" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4852,28 +4853,28 @@
     </row>
     <row r="21" ht="18.0" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="B21" s="137" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="143">
+      <c r="B21" s="138" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="144">
         <f t="shared" si="2"/>
         <v>45542</v>
       </c>
-      <c r="D21" s="139" t="str">
+      <c r="D21" s="140" t="str">
         <f>Timesheet!E30</f>
         <v/>
       </c>
-      <c r="E21" s="144" t="str">
+      <c r="E21" s="145" t="str">
         <f>Timesheet!C30</f>
         <v/>
       </c>
-      <c r="F21" s="145"/>
-      <c r="G21" s="145"/>
-      <c r="H21" s="146"/>
-      <c r="I21" s="141">
+      <c r="F21" s="146"/>
+      <c r="G21" s="146"/>
+      <c r="H21" s="147"/>
+      <c r="I21" s="142">
         <v>50.0</v>
       </c>
-      <c r="J21" s="142">
+      <c r="J21" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4896,28 +4897,28 @@
     </row>
     <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="2"/>
-      <c r="B22" s="137" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="143">
+      <c r="B22" s="138" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="144">
         <f t="shared" si="2"/>
         <v>45543</v>
       </c>
-      <c r="D22" s="139" t="str">
+      <c r="D22" s="140" t="str">
         <f>Timesheet!E33</f>
         <v/>
       </c>
-      <c r="E22" s="144" t="str">
+      <c r="E22" s="145" t="str">
         <f>Timesheet!C33</f>
         <v/>
       </c>
-      <c r="F22" s="145"/>
-      <c r="G22" s="145"/>
-      <c r="H22" s="146"/>
-      <c r="I22" s="141">
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="147"/>
+      <c r="I22" s="142">
         <v>50.0</v>
       </c>
-      <c r="J22" s="142">
+      <c r="J22" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4940,34 +4941,34 @@
     </row>
     <row r="23" ht="26.25" customHeight="1">
       <c r="A23" s="2"/>
-      <c r="B23" s="137" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="138">
+      <c r="B23" s="138" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="139">
         <f t="shared" si="2"/>
         <v>45544</v>
       </c>
-      <c r="D23" s="139" t="str">
+      <c r="D23" s="140" t="str">
         <f>Timesheet!J15</f>
         <v/>
       </c>
-      <c r="E23" s="147" t="str">
+      <c r="E23" s="148" t="str">
         <f>Timesheet!I15</f>
         <v/>
       </c>
-      <c r="F23" s="148"/>
-      <c r="G23" s="148"/>
-      <c r="H23" s="149"/>
-      <c r="I23" s="141">
+      <c r="F23" s="149"/>
+      <c r="G23" s="149"/>
+      <c r="H23" s="150"/>
+      <c r="I23" s="142">
         <v>50.0</v>
       </c>
-      <c r="J23" s="142">
+      <c r="J23" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -4986,28 +4987,28 @@
     </row>
     <row r="24" ht="19.5" customHeight="1">
       <c r="A24" s="2"/>
-      <c r="B24" s="137" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="138">
+      <c r="B24" s="138" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="139">
         <f t="shared" si="2"/>
         <v>45545</v>
       </c>
-      <c r="D24" s="139" t="str">
+      <c r="D24" s="140" t="str">
         <f>Timesheet!J18</f>
         <v/>
       </c>
-      <c r="E24" s="147" t="str">
+      <c r="E24" s="148" t="str">
         <f>Timesheet!I18</f>
         <v/>
       </c>
-      <c r="F24" s="148"/>
-      <c r="G24" s="148"/>
-      <c r="H24" s="149"/>
-      <c r="I24" s="141">
+      <c r="F24" s="149"/>
+      <c r="G24" s="149"/>
+      <c r="H24" s="150"/>
+      <c r="I24" s="142">
         <v>50.0</v>
       </c>
-      <c r="J24" s="142">
+      <c r="J24" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5030,28 +5031,28 @@
     </row>
     <row r="25" ht="33.75" customHeight="1">
       <c r="A25" s="2"/>
-      <c r="B25" s="137" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="138">
+      <c r="B25" s="138" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="139">
         <f t="shared" si="2"/>
         <v>45546</v>
       </c>
-      <c r="D25" s="139" t="str">
+      <c r="D25" s="140" t="str">
         <f>Timesheet!J21</f>
         <v/>
       </c>
-      <c r="E25" s="147" t="str">
+      <c r="E25" s="148" t="str">
         <f>Timesheet!I21</f>
         <v/>
       </c>
-      <c r="F25" s="148"/>
-      <c r="G25" s="148"/>
-      <c r="H25" s="149"/>
-      <c r="I25" s="141">
+      <c r="F25" s="149"/>
+      <c r="G25" s="149"/>
+      <c r="H25" s="150"/>
+      <c r="I25" s="142">
         <v>50.0</v>
       </c>
-      <c r="J25" s="142">
+      <c r="J25" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5074,28 +5075,28 @@
     </row>
     <row r="26" ht="22.5" customHeight="1">
       <c r="A26" s="2"/>
-      <c r="B26" s="137" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="138">
+      <c r="B26" s="138" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="139">
         <f t="shared" si="2"/>
         <v>45547</v>
       </c>
-      <c r="D26" s="139" t="str">
+      <c r="D26" s="140" t="str">
         <f>Timesheet!J24</f>
         <v/>
       </c>
-      <c r="E26" s="147" t="str">
+      <c r="E26" s="148" t="str">
         <f>Timesheet!I24</f>
         <v/>
       </c>
-      <c r="F26" s="148"/>
-      <c r="G26" s="148"/>
-      <c r="H26" s="149"/>
-      <c r="I26" s="141">
+      <c r="F26" s="149"/>
+      <c r="G26" s="149"/>
+      <c r="H26" s="150"/>
+      <c r="I26" s="142">
         <v>50.0</v>
       </c>
-      <c r="J26" s="142">
+      <c r="J26" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5118,28 +5119,28 @@
     </row>
     <row r="27" ht="22.5" customHeight="1">
       <c r="A27" s="2"/>
-      <c r="B27" s="137" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="138">
+      <c r="B27" s="138" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="139">
         <f t="shared" si="2"/>
         <v>45548</v>
       </c>
-      <c r="D27" s="139" t="str">
+      <c r="D27" s="140" t="str">
         <f>Timesheet!J27</f>
         <v/>
       </c>
-      <c r="E27" s="147" t="str">
+      <c r="E27" s="148" t="str">
         <f>Timesheet!I27</f>
         <v/>
       </c>
-      <c r="F27" s="148"/>
-      <c r="G27" s="148"/>
-      <c r="H27" s="149"/>
-      <c r="I27" s="141">
+      <c r="F27" s="149"/>
+      <c r="G27" s="149"/>
+      <c r="H27" s="150"/>
+      <c r="I27" s="142">
         <v>50.0</v>
       </c>
-      <c r="J27" s="142">
+      <c r="J27" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5162,28 +5163,28 @@
     </row>
     <row r="28" ht="18.0" customHeight="1">
       <c r="A28" s="2"/>
-      <c r="B28" s="137" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="143">
+      <c r="B28" s="138" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="144">
         <f t="shared" si="2"/>
         <v>45549</v>
       </c>
-      <c r="D28" s="139" t="str">
+      <c r="D28" s="140" t="str">
         <f>Timesheet!J30</f>
         <v/>
       </c>
-      <c r="E28" s="150" t="str">
+      <c r="E28" s="151" t="str">
         <f>Timesheet!I30</f>
         <v/>
       </c>
-      <c r="F28" s="151"/>
-      <c r="G28" s="151"/>
-      <c r="H28" s="152"/>
-      <c r="I28" s="141">
+      <c r="F28" s="152"/>
+      <c r="G28" s="152"/>
+      <c r="H28" s="153"/>
+      <c r="I28" s="142">
         <v>50.0</v>
       </c>
-      <c r="J28" s="142">
+      <c r="J28" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5206,28 +5207,28 @@
     </row>
     <row r="29" ht="18.0" customHeight="1">
       <c r="A29" s="2"/>
-      <c r="B29" s="137" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="143">
+      <c r="B29" s="138" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="144">
         <f t="shared" si="2"/>
         <v>45550</v>
       </c>
-      <c r="D29" s="139" t="str">
+      <c r="D29" s="140" t="str">
         <f>Timesheet!J33</f>
         <v/>
       </c>
-      <c r="E29" s="150" t="str">
+      <c r="E29" s="151" t="str">
         <f>Timesheet!I33</f>
         <v/>
       </c>
-      <c r="F29" s="151"/>
-      <c r="G29" s="151"/>
-      <c r="H29" s="152"/>
-      <c r="I29" s="141">
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
+      <c r="H29" s="153"/>
+      <c r="I29" s="142">
         <v>50.0</v>
       </c>
-      <c r="J29" s="142">
+      <c r="J29" s="143">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5250,23 +5251,23 @@
     </row>
     <row r="30" ht="18.75" customHeight="1">
       <c r="A30" s="2"/>
-      <c r="B30" s="153"/>
-      <c r="C30" s="153"/>
-      <c r="D30" s="154">
+      <c r="B30" s="154"/>
+      <c r="C30" s="154"/>
+      <c r="D30" s="155">
         <f>SUM(D16:D29)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="155" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="156"/>
-      <c r="G30" s="156"/>
-      <c r="H30" s="157"/>
-      <c r="I30" s="158">
+      <c r="E30" s="156" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="157"/>
+      <c r="G30" s="157"/>
+      <c r="H30" s="158"/>
+      <c r="I30" s="159">
         <f>SUM(D16:D29)</f>
         <v>0</v>
       </c>
-      <c r="J30" s="159"/>
+      <c r="J30" s="160"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -5288,20 +5289,20 @@
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="128"/>
-      <c r="E31" s="160"/>
+      <c r="D31" s="129"/>
+      <c r="E31" s="161"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="161" t="s">
-        <v>58</v>
-      </c>
-      <c r="J31" s="162">
+      <c r="I31" s="162" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" s="163">
         <f>SUM(J16:J29)</f>
         <v>0</v>
       </c>
       <c r="K31" s="2"/>
-      <c r="L31" s="115"/>
+      <c r="L31" s="116"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -5321,18 +5322,18 @@
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="163" t="s">
-        <v>59</v>
-      </c>
-      <c r="G32" s="164" t="str">
+      <c r="D32" s="164" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="165" t="str">
         <f>Timesheet!C7</f>
-        <v>Ricardo Rios</v>
+        <v/>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="165"/>
-      <c r="J32" s="166"/>
+      <c r="I32" s="166"/>
+      <c r="J32" s="167"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="115"/>
+      <c r="L32" s="116"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5352,13 +5353,13 @@
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="167"/>
-      <c r="E33" s="168"/>
-      <c r="F33" s="168"/>
-      <c r="G33" s="168"/>
-      <c r="H33" s="169"/>
-      <c r="I33" s="161"/>
-      <c r="J33" s="166"/>
+      <c r="D33" s="168"/>
+      <c r="E33" s="169"/>
+      <c r="F33" s="169"/>
+      <c r="G33" s="169"/>
+      <c r="H33" s="170"/>
+      <c r="I33" s="162"/>
+      <c r="J33" s="167"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -5380,15 +5381,15 @@
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="170"/>
-      <c r="E34" s="169"/>
-      <c r="F34" s="169"/>
-      <c r="G34" s="169"/>
-      <c r="H34" s="169"/>
-      <c r="I34" s="161" t="s">
-        <v>60</v>
-      </c>
-      <c r="J34" s="171">
+      <c r="D34" s="171"/>
+      <c r="E34" s="170"/>
+      <c r="F34" s="170"/>
+      <c r="G34" s="170"/>
+      <c r="H34" s="170"/>
+      <c r="I34" s="162" t="s">
+        <v>59</v>
+      </c>
+      <c r="J34" s="172">
         <f>J31-J32+J33</f>
         <v>0</v>
       </c>
@@ -5413,13 +5414,13 @@
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="172"/>
-      <c r="E35" s="173"/>
-      <c r="F35" s="174"/>
-      <c r="G35" s="173"/>
-      <c r="H35" s="169"/>
-      <c r="I35" s="175"/>
-      <c r="J35" s="115"/>
+      <c r="D35" s="173"/>
+      <c r="E35" s="174"/>
+      <c r="F35" s="175"/>
+      <c r="G35" s="174"/>
+      <c r="H35" s="170"/>
+      <c r="I35" s="176"/>
+      <c r="J35" s="116"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
@@ -5438,27 +5439,27 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="D36" s="176" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" s="177"/>
-      <c r="F36" s="177"/>
-      <c r="G36" s="177"/>
-      <c r="H36" s="111"/>
-      <c r="I36" s="127"/>
-      <c r="J36" s="129"/>
+      <c r="D36" s="177" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="178"/>
+      <c r="F36" s="178"/>
+      <c r="G36" s="178"/>
+      <c r="H36" s="112"/>
+      <c r="I36" s="128"/>
+      <c r="J36" s="130"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="178"/>
-      <c r="E37" s="178"/>
-      <c r="F37" s="178"/>
-      <c r="G37" s="178"/>
-      <c r="H37" s="178"/>
-      <c r="I37" s="179"/>
-      <c r="J37" s="179"/>
+      <c r="D37" s="179"/>
+      <c r="E37" s="179"/>
+      <c r="F37" s="179"/>
+      <c r="G37" s="179"/>
+      <c r="H37" s="179"/>
+      <c r="I37" s="180"/>
+      <c r="J37" s="180"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
@@ -5483,16 +5484,16 @@
       <c r="G38" s="2"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="D39" s="180"/>
-      <c r="E39" s="181"/>
-      <c r="F39" s="181"/>
-      <c r="G39" s="181"/>
+      <c r="D39" s="181"/>
+      <c r="E39" s="182"/>
+      <c r="F39" s="182"/>
+      <c r="G39" s="182"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="D40" s="176"/>
-      <c r="E40" s="177"/>
-      <c r="F40" s="177"/>
-      <c r="G40" s="177"/>
+      <c r="D40" s="177"/>
+      <c r="E40" s="178"/>
+      <c r="F40" s="178"/>
+      <c r="G40" s="178"/>
     </row>
     <row r="41" ht="12.75" customHeight="1"/>
     <row r="42" ht="12.75" customHeight="1"/>

</xml_diff>